<commit_message>
Pushed new files and file updates
</commit_message>
<xml_diff>
--- a/Documentation/EEOB563_Final_Project_Scores_Reference_and_Tables_Setup.xlsx
+++ b/Documentation/EEOB563_Final_Project_Scores_Reference_and_Tables_Setup.xlsx
@@ -1683,7 +1683,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="203">
+  <cellStyleXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1887,8 +1887,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1982,6 +1986,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1997,24 +2047,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90"/>
     </xf>
@@ -2024,15 +2056,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2042,66 +2074,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="203">
+  <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2203,6 +2192,8 @@
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2304,6 +2295,8 @@
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4707,40 +4700,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="63" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="63" t="s">
         <v>318</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="63" t="s">
         <v>319</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="47"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="67"/>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="15" thickBot="1">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="11" t="s">
         <v>143</v>
       </c>
@@ -4797,7 +4790,7 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="60" t="s">
         <v>322</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -4862,7 +4855,7 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="49"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="21" t="s">
         <v>325</v>
       </c>
@@ -4925,7 +4918,7 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="49"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="21" t="s">
         <v>327</v>
       </c>
@@ -4988,7 +4981,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1">
-      <c r="A6" s="53"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="24" t="s">
         <v>329</v>
       </c>
@@ -5051,7 +5044,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="14" customHeight="1">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="62" t="s">
         <v>331</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -5116,7 +5109,7 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="49"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="21" t="s">
         <v>325</v>
       </c>
@@ -5179,7 +5172,7 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="49"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="21" t="s">
         <v>334</v>
       </c>
@@ -5242,7 +5235,7 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="49"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="21" t="s">
         <v>327</v>
       </c>
@@ -5305,7 +5298,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1">
-      <c r="A11" s="53"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="24" t="s">
         <v>329</v>
       </c>
@@ -5368,7 +5361,7 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="62" t="s">
         <v>338</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -5433,7 +5426,7 @@
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="49"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="21" t="s">
         <v>340</v>
       </c>
@@ -5496,7 +5489,7 @@
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="49"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="21" t="s">
         <v>342</v>
       </c>
@@ -5559,7 +5552,7 @@
       </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="49"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="21" t="s">
         <v>344</v>
       </c>
@@ -5622,7 +5615,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" thickBot="1">
-      <c r="A16" s="53"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="24" t="s">
         <v>346</v>
       </c>
@@ -5685,7 +5678,7 @@
       </c>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="62" t="s">
         <v>348</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -5750,7 +5743,7 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="49"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="21" t="s">
         <v>350</v>
       </c>
@@ -5813,7 +5806,7 @@
       </c>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="49"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="21" t="s">
         <v>352</v>
       </c>
@@ -5876,7 +5869,7 @@
       </c>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="49"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="21" t="s">
         <v>327</v>
       </c>
@@ -5939,7 +5932,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15" thickBot="1">
-      <c r="A21" s="53"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="24" t="s">
         <v>329</v>
       </c>
@@ -6002,7 +5995,7 @@
       </c>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="62" t="s">
         <v>356</v>
       </c>
       <c r="B22" s="25" t="s">
@@ -6067,7 +6060,7 @@
       </c>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="49"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="21" t="s">
         <v>352</v>
       </c>
@@ -6130,7 +6123,7 @@
       </c>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="49"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="21" t="s">
         <v>359</v>
       </c>
@@ -6193,7 +6186,7 @@
       </c>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="49"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="21" t="s">
         <v>327</v>
       </c>
@@ -6256,7 +6249,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" thickBot="1">
-      <c r="A26" s="53"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="24" t="s">
         <v>329</v>
       </c>
@@ -6319,7 +6312,7 @@
       </c>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="62" t="s">
         <v>363</v>
       </c>
       <c r="B27" s="25" t="s">
@@ -6384,7 +6377,7 @@
       </c>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="49"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="21" t="s">
         <v>365</v>
       </c>
@@ -6447,7 +6440,7 @@
       </c>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="49"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="21" t="s">
         <v>367</v>
       </c>
@@ -6510,7 +6503,7 @@
       </c>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="49"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="21" t="s">
         <v>369</v>
       </c>
@@ -6573,7 +6566,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="15" thickBot="1">
-      <c r="A31" s="53"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="24" t="s">
         <v>371</v>
       </c>
@@ -6636,7 +6629,7 @@
       </c>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="62" t="s">
         <v>373</v>
       </c>
       <c r="B32" s="16" t="s">
@@ -6701,7 +6694,7 @@
       </c>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="49"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="21" t="s">
         <v>325</v>
       </c>
@@ -6764,7 +6757,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="15" thickBot="1">
-      <c r="A34" s="49"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="21" t="s">
         <v>327</v>
       </c>
@@ -6827,7 +6820,7 @@
       </c>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="50" t="s">
+      <c r="A35" s="57" t="s">
         <v>377</v>
       </c>
       <c r="B35" s="27" t="s">
@@ -6892,7 +6885,7 @@
       </c>
     </row>
     <row r="36" spans="1:21">
-      <c r="A36" s="51"/>
+      <c r="A36" s="58"/>
       <c r="B36" s="28" t="s">
         <v>380</v>
       </c>
@@ -6955,7 +6948,7 @@
       </c>
     </row>
     <row r="37" spans="1:21">
-      <c r="A37" s="51"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="28" t="s">
         <v>382</v>
       </c>
@@ -7018,7 +7011,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="15" thickBot="1">
-      <c r="A38" s="52"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="29" t="s">
         <v>384</v>
       </c>
@@ -7082,6 +7075,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:U1"/>
+    <mergeCell ref="A32:A34"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A11"/>
@@ -7089,11 +7087,6 @@
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:U1"/>
-    <mergeCell ref="A32:A34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7122,10 +7115,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:81" ht="55">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="69" t="s">
         <v>386</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="68" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="35"/>
@@ -7166,8 +7159,8 @@
       <c r="BK4" s="3"/>
     </row>
     <row r="5" spans="2:81" ht="155">
-      <c r="B5" s="55"/>
-      <c r="C5" s="54"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="35" t="s">
         <v>238</v>
       </c>
@@ -7228,7 +7221,7 @@
       <c r="BG5" s="33"/>
       <c r="BH5" s="33"/>
       <c r="BI5" s="33"/>
-      <c r="BJ5" s="56" t="s">
+      <c r="BJ5" s="70" t="s">
         <v>388</v>
       </c>
       <c r="BK5" s="34"/>
@@ -7254,8 +7247,8 @@
       <c r="CC5" s="33"/>
     </row>
     <row r="6" spans="2:81" ht="182">
-      <c r="B6" s="55"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="68"/>
       <c r="D6" s="35" t="s">
         <v>193</v>
       </c>
@@ -7302,7 +7295,7 @@
       <c r="AI6" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="AL6" s="56" t="s">
+      <c r="AL6" s="70" t="s">
         <v>387</v>
       </c>
       <c r="AM6" s="34"/>
@@ -7340,7 +7333,7 @@
       <c r="BG6" s="33"/>
       <c r="BH6" s="33"/>
       <c r="BI6" s="33"/>
-      <c r="BJ6" s="56"/>
+      <c r="BJ6" s="70"/>
       <c r="BK6" s="34"/>
       <c r="BL6" s="33" t="s">
         <v>274</v>
@@ -7372,8 +7365,8 @@
       <c r="CC6" s="33"/>
     </row>
     <row r="7" spans="2:81" ht="178">
-      <c r="B7" s="55"/>
-      <c r="C7" s="54"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="68"/>
       <c r="D7" s="36" t="s">
         <v>191</v>
       </c>
@@ -7436,7 +7429,7 @@
       <c r="AI7" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="AL7" s="56"/>
+      <c r="AL7" s="70"/>
       <c r="AM7" s="34"/>
       <c r="AN7" s="33" t="s">
         <v>75</v>
@@ -7492,7 +7485,7 @@
       </c>
       <c r="BH7" s="33"/>
       <c r="BI7" s="33"/>
-      <c r="BJ7" s="56"/>
+      <c r="BJ7" s="70"/>
       <c r="BK7" s="34"/>
       <c r="BL7" s="33" t="s">
         <v>273</v>
@@ -7546,8 +7539,8 @@
       </c>
     </row>
     <row r="8" spans="2:81" ht="192">
-      <c r="B8" s="55"/>
-      <c r="C8" s="54"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="36" t="s">
         <v>189</v>
       </c>
@@ -7628,7 +7621,7 @@
       <c r="AI8" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="AL8" s="56"/>
+      <c r="AL8" s="70"/>
       <c r="AM8" s="34"/>
       <c r="AN8" s="33" t="s">
         <v>74</v>
@@ -7692,7 +7685,7 @@
       </c>
       <c r="BH8" s="33"/>
       <c r="BI8" s="33"/>
-      <c r="BJ8" s="56"/>
+      <c r="BJ8" s="70"/>
       <c r="BK8" s="34"/>
       <c r="BL8" s="33" t="s">
         <v>272</v>
@@ -7750,8 +7743,8 @@
       </c>
     </row>
     <row r="9" spans="2:81" ht="187">
-      <c r="B9" s="55"/>
-      <c r="C9" s="54"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="35" t="s">
         <v>190</v>
       </c>
@@ -7848,7 +7841,7 @@
       <c r="AI9" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="AL9" s="56"/>
+      <c r="AL9" s="70"/>
       <c r="AM9" s="34"/>
       <c r="AN9" s="33" t="s">
         <v>73</v>
@@ -7912,7 +7905,7 @@
       </c>
       <c r="BH9" s="33"/>
       <c r="BI9" s="33"/>
-      <c r="BJ9" s="56"/>
+      <c r="BJ9" s="70"/>
       <c r="BK9" s="34"/>
       <c r="BL9" s="33" t="s">
         <v>271</v>
@@ -7970,8 +7963,8 @@
       </c>
     </row>
     <row r="10" spans="2:81" ht="190">
-      <c r="B10" s="55"/>
-      <c r="C10" s="54"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="35" t="s">
         <v>192</v>
       </c>
@@ -8068,7 +8061,7 @@
       <c r="AI10" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="AL10" s="56"/>
+      <c r="AL10" s="70"/>
       <c r="AM10" s="34" t="s">
         <v>1</v>
       </c>
@@ -8134,7 +8127,7 @@
       </c>
       <c r="BH10" s="33"/>
       <c r="BI10" s="33"/>
-      <c r="BJ10" s="56"/>
+      <c r="BJ10" s="70"/>
       <c r="BK10" s="34" t="s">
         <v>1</v>
       </c>
@@ -8194,7 +8187,7 @@
       </c>
     </row>
     <row r="11" spans="2:81" ht="129">
-      <c r="B11" s="55"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="39" t="s">
         <v>0</v>
       </c>
@@ -8294,7 +8287,7 @@
       <c r="AI11" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="AL11" s="56"/>
+      <c r="AL11" s="70"/>
       <c r="AM11" s="34" t="s">
         <v>72</v>
       </c>
@@ -8360,7 +8353,7 @@
       </c>
       <c r="BH11" s="33"/>
       <c r="BI11" s="33"/>
-      <c r="BJ11" s="56"/>
+      <c r="BJ11" s="70"/>
       <c r="BK11" s="34" t="s">
         <v>142</v>
       </c>
@@ -8466,18 +8459,23 @@
   <dimension ref="A2:AE58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="6.83203125" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" customWidth="1"/>
-    <col min="4" max="4" width="52.83203125" style="57" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="52.83203125" style="43" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="13" width="8.83203125" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" customWidth="1"/>
+    <col min="16" max="16" width="9.83203125" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" customWidth="1"/>
+    <col min="18" max="18" width="9.83203125" customWidth="1"/>
     <col min="21" max="22" width="4.83203125" customWidth="1"/>
     <col min="23" max="25" width="2.83203125" customWidth="1"/>
     <col min="26" max="31" width="6.83203125" customWidth="1"/>
@@ -8497,205 +8495,205 @@
     </row>
     <row r="4" spans="1:18" ht="14" customHeight="1">
       <c r="A4" s="3"/>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="74" t="s">
         <v>317</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="74" t="s">
         <v>389</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="79" t="s">
         <v>427</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="79" t="s">
+      <c r="H4" s="73" t="s">
         <v>432</v>
       </c>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="73" t="s">
         <v>433</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="73" t="s">
         <v>434</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="73" t="s">
         <v>435</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="73" t="s">
         <v>436</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="73" t="s">
         <v>437</v>
       </c>
-      <c r="N4" s="78" t="s">
+      <c r="N4" s="73" t="s">
         <v>438</v>
       </c>
-      <c r="O4" s="78" t="s">
+      <c r="O4" s="73" t="s">
         <v>444</v>
       </c>
-      <c r="P4" s="75" t="s">
+      <c r="P4" s="73" t="s">
         <v>448</v>
       </c>
-      <c r="Q4" s="75" t="s">
+      <c r="Q4" s="73" t="s">
         <v>440</v>
       </c>
-      <c r="R4" s="75" t="s">
+      <c r="R4" s="73" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="73"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="80"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
     </row>
     <row r="6" spans="1:18" ht="14" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="76" t="s">
         <v>322</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="47" t="s">
         <v>324</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="D6" s="48" t="s">
         <v>391</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="73" t="s">
         <v>428</v>
       </c>
-      <c r="I6" s="78" t="s">
+      <c r="I6" s="73" t="s">
         <v>439</v>
       </c>
-      <c r="J6" s="74">
+      <c r="J6" s="73">
         <v>-2544.782224</v>
       </c>
-      <c r="K6" s="74">
+      <c r="K6" s="73">
         <v>5227.5644490000004</v>
       </c>
-      <c r="L6" s="74">
+      <c r="L6" s="73">
         <v>14887.564449</v>
       </c>
-      <c r="M6" s="74">
+      <c r="M6" s="73">
         <v>5382.7106199999998</v>
       </c>
-      <c r="N6" s="74">
+      <c r="N6" s="73">
         <v>69</v>
       </c>
-      <c r="O6" s="78">
+      <c r="O6" s="73">
         <v>70</v>
       </c>
-      <c r="P6" s="78" t="s">
+      <c r="P6" s="73" t="s">
         <v>442</v>
       </c>
-      <c r="Q6" s="78" t="s">
+      <c r="Q6" s="73" t="s">
         <v>443</v>
       </c>
-      <c r="R6" s="78" t="s">
+      <c r="R6" s="73" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="3"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59" t="s">
+      <c r="B7" s="77"/>
+      <c r="C7" s="44" t="s">
         <v>326</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="45" t="s">
         <v>392</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="78"/>
-      <c r="R7" s="78"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="3"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="59" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="45" t="s">
         <v>393</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-    </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1">
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+    </row>
+    <row r="9" spans="1:18" ht="29" thickBot="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="68" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="49" t="s">
         <v>330</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="50" t="s">
         <v>394</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="53" t="s">
         <v>429</v>
       </c>
-      <c r="I9" s="77" t="s">
+      <c r="I9" s="53" t="s">
         <v>381</v>
       </c>
-      <c r="J9" s="77">
+      <c r="J9" s="53">
         <v>-636.42025799999999</v>
       </c>
-      <c r="K9" s="77">
+      <c r="K9" s="53">
         <v>1398.8405170000001</v>
       </c>
-      <c r="L9" s="77">
+      <c r="L9" s="53">
         <v>9462.8405170000005</v>
       </c>
-      <c r="M9" s="77">
+      <c r="M9" s="53">
         <v>1491.1818780000001</v>
       </c>
-      <c r="N9" s="77">
+      <c r="N9" s="53">
         <v>63</v>
       </c>
-      <c r="O9" s="80">
+      <c r="O9" s="53">
         <v>32</v>
       </c>
-      <c r="P9" s="77" t="s">
+      <c r="P9" s="53" t="s">
         <v>442</v>
       </c>
       <c r="Q9" s="81" t="s">
@@ -8705,24 +8703,24 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" ht="28">
       <c r="A10" s="3"/>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="76" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="47" t="s">
         <v>332</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="48" t="s">
         <v>395</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="76" t="s">
+      <c r="H10" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="I10" s="77" t="s">
+      <c r="I10" s="53" t="s">
         <v>381</v>
       </c>
       <c r="J10" s="81" t="s">
@@ -8753,110 +8751,110 @@
         <v>445</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="28">
       <c r="A11" s="3"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="44" t="s">
         <v>333</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="45" t="s">
         <v>396</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="76" t="s">
+      <c r="H11" s="53" t="s">
         <v>431</v>
       </c>
-      <c r="I11" s="77" t="s">
+      <c r="I11" s="53" t="s">
         <v>381</v>
       </c>
-      <c r="J11" s="77">
+      <c r="J11" s="53">
         <v>-639.63207399999999</v>
       </c>
-      <c r="K11" s="77">
+      <c r="K11" s="53">
         <v>1405.2641490000001</v>
       </c>
-      <c r="L11" s="77">
+      <c r="L11" s="53">
         <v>9469.2641490000005</v>
       </c>
-      <c r="M11" s="77">
+      <c r="M11" s="53">
         <v>1461.357569</v>
       </c>
-      <c r="N11" s="77">
+      <c r="N11" s="53">
         <v>63</v>
       </c>
-      <c r="O11" s="80">
+      <c r="O11" s="53">
         <v>18</v>
       </c>
-      <c r="P11" s="77" t="s">
+      <c r="P11" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="Q11" s="77" t="s">
+      <c r="Q11" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="R11" s="77" t="s">
+      <c r="R11" s="53" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="28">
       <c r="A12" s="3"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="59" t="s">
+      <c r="B12" s="77"/>
+      <c r="C12" s="44" t="s">
         <v>335</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="45" t="s">
         <v>397</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="76" t="s">
+      <c r="H12" s="53" t="s">
         <v>429</v>
       </c>
-      <c r="I12" s="77" t="s">
+      <c r="I12" s="53" t="s">
         <v>379</v>
       </c>
-      <c r="J12" s="77">
+      <c r="J12" s="53">
         <v>-627.05075399999998</v>
       </c>
-      <c r="K12" s="77">
+      <c r="K12" s="53">
         <v>1380.1015070000001</v>
       </c>
-      <c r="L12" s="77">
+      <c r="L12" s="53">
         <v>9444.1015069999994</v>
       </c>
-      <c r="M12" s="77">
+      <c r="M12" s="53">
         <v>1472.442869</v>
       </c>
-      <c r="N12" s="77">
+      <c r="N12" s="53">
         <v>63</v>
       </c>
-      <c r="O12" s="80">
+      <c r="O12" s="53">
         <v>32</v>
       </c>
-      <c r="P12" s="77" t="s">
+      <c r="P12" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="Q12" s="77" t="s">
+      <c r="Q12" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="R12" s="77" t="s">
+      <c r="R12" s="53" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
-      <c r="B13" s="58"/>
-      <c r="C13" s="59" t="s">
+    <row r="13" spans="1:18" ht="28">
+      <c r="B13" s="77"/>
+      <c r="C13" s="44" t="s">
         <v>336</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="45" t="s">
         <v>398</v>
       </c>
-      <c r="H13" s="76" t="s">
+      <c r="H13" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="I13" s="77" t="s">
+      <c r="I13" s="53" t="s">
         <v>379</v>
       </c>
       <c r="J13" s="81" t="s">
@@ -8887,643 +8885,647 @@
         <v>445</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1">
-      <c r="B14" s="67"/>
-      <c r="C14" s="68" t="s">
+    <row r="14" spans="1:18" ht="29" thickBot="1">
+      <c r="B14" s="78"/>
+      <c r="C14" s="49" t="s">
         <v>337</v>
       </c>
-      <c r="D14" s="69" t="s">
+      <c r="D14" s="50" t="s">
         <v>399</v>
       </c>
-      <c r="H14" s="76" t="s">
+      <c r="H14" s="53" t="s">
         <v>431</v>
       </c>
-      <c r="I14" s="77" t="s">
+      <c r="I14" s="53" t="s">
         <v>379</v>
       </c>
-      <c r="J14" s="77">
+      <c r="J14" s="53">
         <v>-632.35218199999997</v>
       </c>
-      <c r="K14" s="77">
+      <c r="K14" s="53">
         <v>1390.7043639999999</v>
       </c>
-      <c r="L14" s="77">
+      <c r="L14" s="53">
         <v>9454.7043639999993</v>
       </c>
-      <c r="M14" s="77">
+      <c r="M14" s="53">
         <v>1446.797785</v>
       </c>
-      <c r="N14" s="77">
+      <c r="N14" s="53">
         <v>63</v>
       </c>
-      <c r="O14" s="80">
+      <c r="O14" s="53">
         <v>18</v>
       </c>
-      <c r="P14" s="77" t="s">
+      <c r="P14" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="Q14" s="77" t="s">
+      <c r="Q14" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="R14" s="77" t="s">
+      <c r="R14" s="53" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="76" t="s">
         <v>338</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="47" t="s">
         <v>339</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="48" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="B16" s="58"/>
-      <c r="C16" s="59" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="45" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="58"/>
-      <c r="C17" s="59" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="45" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="58"/>
-      <c r="C18" s="59" t="s">
+      <c r="B18" s="77"/>
+      <c r="C18" s="44" t="s">
         <v>345</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="45" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15" thickBot="1">
-      <c r="B19" s="67"/>
-      <c r="C19" s="68" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="49" t="s">
         <v>347</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D19" s="50" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="76" t="s">
         <v>348</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="48" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="58"/>
-      <c r="C21" s="59" t="s">
+      <c r="B21" s="77"/>
+      <c r="C21" s="44" t="s">
         <v>351</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="45" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="58"/>
-      <c r="C22" s="59" t="s">
+      <c r="B22" s="77"/>
+      <c r="C22" s="44" t="s">
         <v>353</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="45" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="58"/>
-      <c r="C23" s="59" t="s">
+      <c r="B23" s="77"/>
+      <c r="C23" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="45" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15" thickBot="1">
-      <c r="B24" s="67"/>
-      <c r="C24" s="68" t="s">
+      <c r="B24" s="78"/>
+      <c r="C24" s="49" t="s">
         <v>355</v>
       </c>
-      <c r="D24" s="69" t="s">
+      <c r="D24" s="50" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="76" t="s">
         <v>356</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="47" t="s">
         <v>357</v>
       </c>
-      <c r="D25" s="66" t="s">
+      <c r="D25" s="48" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="58"/>
-      <c r="C26" s="59" t="s">
+      <c r="B26" s="77"/>
+      <c r="C26" s="44" t="s">
         <v>358</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="45" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="58"/>
-      <c r="C27" s="59" t="s">
+      <c r="B27" s="77"/>
+      <c r="C27" s="44" t="s">
         <v>360</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="45" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="58"/>
-      <c r="C28" s="59" t="s">
+      <c r="B28" s="77"/>
+      <c r="C28" s="44" t="s">
         <v>361</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="45" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="15" thickBot="1">
-      <c r="B29" s="67"/>
-      <c r="C29" s="68" t="s">
+      <c r="B29" s="78"/>
+      <c r="C29" s="49" t="s">
         <v>362</v>
       </c>
-      <c r="D29" s="69" t="s">
+      <c r="D29" s="50" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="76" t="s">
         <v>390</v>
       </c>
-      <c r="C30" s="65" t="s">
+      <c r="C30" s="47" t="s">
         <v>364</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="48" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="58"/>
-      <c r="C31" s="59" t="s">
+      <c r="B31" s="77"/>
+      <c r="C31" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="D31" s="60" t="s">
+      <c r="D31" s="45" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="58"/>
-      <c r="C32" s="59" t="s">
+      <c r="B32" s="77"/>
+      <c r="C32" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="45" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="33" spans="2:31">
-      <c r="B33" s="58"/>
-      <c r="C33" s="59" t="s">
+      <c r="B33" s="77"/>
+      <c r="C33" s="44" t="s">
         <v>370</v>
       </c>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="45" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="34" spans="2:31" ht="15" thickBot="1">
-      <c r="B34" s="67"/>
-      <c r="C34" s="68" t="s">
+      <c r="B34" s="78"/>
+      <c r="C34" s="49" t="s">
         <v>372</v>
       </c>
-      <c r="D34" s="69" t="s">
+      <c r="D34" s="50" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="35" spans="2:31">
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="76" t="s">
         <v>373</v>
       </c>
-      <c r="C35" s="65" t="s">
+      <c r="C35" s="47" t="s">
         <v>374</v>
       </c>
-      <c r="D35" s="66" t="s">
+      <c r="D35" s="48" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="36" spans="2:31">
-      <c r="B36" s="58"/>
-      <c r="C36" s="59" t="s">
+      <c r="B36" s="77"/>
+      <c r="C36" s="44" t="s">
         <v>375</v>
       </c>
-      <c r="D36" s="60" t="s">
+      <c r="D36" s="45" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="37" spans="2:31" ht="15" thickBot="1">
-      <c r="B37" s="67"/>
-      <c r="C37" s="68" t="s">
+      <c r="B37" s="78"/>
+      <c r="C37" s="49" t="s">
         <v>376</v>
       </c>
-      <c r="D37" s="69" t="s">
+      <c r="D37" s="50" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="38" spans="2:31">
-      <c r="B38" s="64" t="s">
+      <c r="B38" s="76" t="s">
         <v>377</v>
       </c>
-      <c r="C38" s="70" t="s">
+      <c r="C38" s="51" t="s">
         <v>379</v>
       </c>
-      <c r="D38" s="66" t="s">
+      <c r="D38" s="48" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="39" spans="2:31">
-      <c r="B39" s="58"/>
-      <c r="C39" s="61" t="s">
+      <c r="B39" s="77"/>
+      <c r="C39" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="45" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="40" spans="2:31">
-      <c r="B40" s="58"/>
-      <c r="C40" s="61" t="s">
+      <c r="B40" s="77"/>
+      <c r="C40" s="46" t="s">
         <v>383</v>
       </c>
-      <c r="D40" s="60" t="s">
+      <c r="D40" s="45" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="41" spans="2:31" ht="15" thickBot="1">
-      <c r="B41" s="67"/>
-      <c r="C41" s="71" t="s">
+      <c r="B41" s="78"/>
+      <c r="C41" s="52" t="s">
         <v>385</v>
       </c>
-      <c r="D41" s="69" t="s">
+      <c r="D41" s="50" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="48" spans="2:31" ht="59" customHeight="1">
-      <c r="U48" s="82" t="s">
+      <c r="U48" s="71" t="s">
         <v>441</v>
       </c>
-      <c r="V48" s="82"/>
-      <c r="W48" s="82" t="s">
+      <c r="V48" s="71"/>
+      <c r="W48" s="71" t="s">
         <v>447</v>
       </c>
-      <c r="X48" s="82"/>
-      <c r="Y48" s="82"/>
-      <c r="Z48" s="83" t="s">
+      <c r="X48" s="71"/>
+      <c r="Y48" s="71"/>
+      <c r="Z48" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AA48" s="83" t="s">
+      <c r="AA48" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB48" s="84" t="s">
+      <c r="AB48" s="55" t="s">
         <v>446</v>
       </c>
-      <c r="AC48" s="84" t="s">
+      <c r="AC48" s="55" t="s">
         <v>446</v>
       </c>
-      <c r="AD48" s="83" t="s">
+      <c r="AD48" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE48" s="84" t="s">
+      <c r="AE48" s="55" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="49" spans="21:31" ht="46" customHeight="1">
-      <c r="U49" s="82" t="s">
+      <c r="U49" s="71" t="s">
         <v>440</v>
       </c>
-      <c r="V49" s="82"/>
-      <c r="W49" s="82" t="s">
+      <c r="V49" s="71"/>
+      <c r="W49" s="71" t="s">
         <v>443</v>
       </c>
-      <c r="X49" s="82"/>
-      <c r="Y49" s="82"/>
-      <c r="Z49" s="83" t="s">
+      <c r="X49" s="71"/>
+      <c r="Y49" s="71"/>
+      <c r="Z49" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AA49" s="83" t="s">
+      <c r="AA49" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB49" s="84" t="s">
+      <c r="AB49" s="55" t="s">
         <v>442</v>
       </c>
-      <c r="AC49" s="84" t="s">
+      <c r="AC49" s="55" t="s">
         <v>442</v>
       </c>
-      <c r="AD49" s="83" t="s">
+      <c r="AD49" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE49" s="84" t="s">
+      <c r="AE49" s="55" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="50" spans="21:31" ht="48" customHeight="1">
-      <c r="U50" s="82" t="s">
+      <c r="U50" s="71" t="s">
         <v>448</v>
       </c>
-      <c r="V50" s="82"/>
-      <c r="W50" s="82" t="s">
+      <c r="V50" s="71"/>
+      <c r="W50" s="71" t="s">
         <v>442</v>
       </c>
-      <c r="X50" s="82"/>
-      <c r="Y50" s="82"/>
-      <c r="Z50" s="84" t="s">
+      <c r="X50" s="71"/>
+      <c r="Y50" s="71"/>
+      <c r="Z50" s="55" t="s">
         <v>442</v>
       </c>
-      <c r="AA50" s="83" t="s">
+      <c r="AA50" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB50" s="84" t="s">
+      <c r="AB50" s="55" t="s">
         <v>442</v>
       </c>
-      <c r="AC50" s="84" t="s">
+      <c r="AC50" s="55" t="s">
         <v>442</v>
       </c>
-      <c r="AD50" s="83" t="s">
+      <c r="AD50" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE50" s="84" t="s">
+      <c r="AE50" s="55" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="51" spans="21:31" ht="48" customHeight="1">
-      <c r="U51" s="82" t="s">
+      <c r="U51" s="71" t="s">
         <v>444</v>
       </c>
-      <c r="V51" s="82"/>
-      <c r="W51" s="82">
+      <c r="V51" s="71"/>
+      <c r="W51" s="71">
         <v>70</v>
       </c>
-      <c r="X51" s="82"/>
-      <c r="Y51" s="82"/>
-      <c r="Z51" s="85">
+      <c r="X51" s="71"/>
+      <c r="Y51" s="71"/>
+      <c r="Z51" s="56">
         <v>32</v>
       </c>
-      <c r="AA51" s="83" t="s">
+      <c r="AA51" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB51" s="85">
+      <c r="AB51" s="56">
         <v>18</v>
       </c>
-      <c r="AC51" s="85">
+      <c r="AC51" s="56">
         <v>32</v>
       </c>
-      <c r="AD51" s="83" t="s">
+      <c r="AD51" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE51" s="85">
+      <c r="AE51" s="56">
         <v>18</v>
       </c>
     </row>
     <row r="52" spans="21:31" ht="73" customHeight="1">
-      <c r="U52" s="82" t="s">
+      <c r="U52" s="71" t="s">
         <v>438</v>
       </c>
-      <c r="V52" s="82"/>
-      <c r="W52" s="86">
+      <c r="V52" s="71"/>
+      <c r="W52" s="72">
         <v>69</v>
       </c>
-      <c r="X52" s="86"/>
-      <c r="Y52" s="86"/>
-      <c r="Z52" s="84">
+      <c r="X52" s="72"/>
+      <c r="Y52" s="72"/>
+      <c r="Z52" s="55">
         <v>63</v>
       </c>
-      <c r="AA52" s="83" t="s">
+      <c r="AA52" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB52" s="84">
+      <c r="AB52" s="55">
         <v>63</v>
       </c>
-      <c r="AC52" s="84">
+      <c r="AC52" s="55">
         <v>63</v>
       </c>
-      <c r="AD52" s="83" t="s">
+      <c r="AD52" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE52" s="84">
+      <c r="AE52" s="55">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="21:31" ht="53" customHeight="1">
-      <c r="U53" s="82" t="s">
+      <c r="U53" s="71" t="s">
         <v>437</v>
       </c>
-      <c r="V53" s="82"/>
-      <c r="W53" s="86">
+      <c r="V53" s="71"/>
+      <c r="W53" s="72">
         <v>5382.7106199999998</v>
       </c>
-      <c r="X53" s="86"/>
-      <c r="Y53" s="86"/>
-      <c r="Z53" s="84">
+      <c r="X53" s="72"/>
+      <c r="Y53" s="72"/>
+      <c r="Z53" s="55">
         <v>1491.1818780000001</v>
       </c>
-      <c r="AA53" s="83" t="s">
+      <c r="AA53" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB53" s="84">
+      <c r="AB53" s="55">
         <v>1461.357569</v>
       </c>
-      <c r="AC53" s="84">
+      <c r="AC53" s="55">
         <v>1472.442869</v>
       </c>
-      <c r="AD53" s="83" t="s">
+      <c r="AD53" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE53" s="84">
+      <c r="AE53" s="55">
         <v>1446.797785</v>
       </c>
     </row>
     <row r="54" spans="21:31" ht="53" customHeight="1">
-      <c r="U54" s="82" t="s">
+      <c r="U54" s="71" t="s">
         <v>436</v>
       </c>
-      <c r="V54" s="82"/>
-      <c r="W54" s="86">
+      <c r="V54" s="71"/>
+      <c r="W54" s="72">
         <v>14887.564449</v>
       </c>
-      <c r="X54" s="86"/>
-      <c r="Y54" s="86"/>
-      <c r="Z54" s="84">
+      <c r="X54" s="72"/>
+      <c r="Y54" s="72"/>
+      <c r="Z54" s="55">
         <v>9462.8405170000005</v>
       </c>
-      <c r="AA54" s="83" t="s">
+      <c r="AA54" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB54" s="84">
+      <c r="AB54" s="55">
         <v>9469.2641490000005</v>
       </c>
-      <c r="AC54" s="84">
+      <c r="AC54" s="55">
         <v>9444.1015069999994</v>
       </c>
-      <c r="AD54" s="83" t="s">
+      <c r="AD54" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE54" s="84">
+      <c r="AE54" s="55">
         <v>9454.7043639999993</v>
       </c>
     </row>
     <row r="55" spans="21:31" ht="53" customHeight="1">
-      <c r="U55" s="82" t="s">
+      <c r="U55" s="71" t="s">
         <v>435</v>
       </c>
-      <c r="V55" s="82"/>
-      <c r="W55" s="86">
+      <c r="V55" s="71"/>
+      <c r="W55" s="72">
         <v>5227.5644490000004</v>
       </c>
-      <c r="X55" s="86"/>
-      <c r="Y55" s="86"/>
-      <c r="Z55" s="84">
+      <c r="X55" s="72"/>
+      <c r="Y55" s="72"/>
+      <c r="Z55" s="55">
         <v>1398.8405170000001</v>
       </c>
-      <c r="AA55" s="83" t="s">
+      <c r="AA55" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB55" s="84">
+      <c r="AB55" s="55">
         <v>1405.2641490000001</v>
       </c>
-      <c r="AC55" s="84">
+      <c r="AC55" s="55">
         <v>1380.1015070000001</v>
       </c>
-      <c r="AD55" s="83" t="s">
+      <c r="AD55" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE55" s="84">
+      <c r="AE55" s="55">
         <v>1390.7043639999999</v>
       </c>
     </row>
     <row r="56" spans="21:31" ht="62" customHeight="1">
-      <c r="U56" s="82" t="s">
+      <c r="U56" s="71" t="s">
         <v>434</v>
       </c>
-      <c r="V56" s="82"/>
-      <c r="W56" s="86">
+      <c r="V56" s="71"/>
+      <c r="W56" s="72">
         <v>-2544.782224</v>
       </c>
-      <c r="X56" s="86"/>
-      <c r="Y56" s="86"/>
-      <c r="Z56" s="84">
+      <c r="X56" s="72"/>
+      <c r="Y56" s="72"/>
+      <c r="Z56" s="55">
         <v>-636.42025799999999</v>
       </c>
-      <c r="AA56" s="83" t="s">
+      <c r="AA56" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AB56" s="84">
+      <c r="AB56" s="55">
         <v>-639.63207399999999</v>
       </c>
-      <c r="AC56" s="84">
+      <c r="AC56" s="55">
         <v>-627.05075399999998</v>
       </c>
-      <c r="AD56" s="83" t="s">
+      <c r="AD56" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="AE56" s="84">
+      <c r="AE56" s="55">
         <v>-632.35218199999997</v>
       </c>
     </row>
     <row r="57" spans="21:31" ht="76" customHeight="1">
-      <c r="U57" s="82" t="s">
+      <c r="U57" s="71" t="s">
         <v>433</v>
       </c>
-      <c r="V57" s="82"/>
-      <c r="W57" s="82" t="s">
+      <c r="V57" s="71"/>
+      <c r="W57" s="71" t="s">
         <v>439</v>
       </c>
-      <c r="X57" s="82"/>
-      <c r="Y57" s="82"/>
-      <c r="Z57" s="84" t="s">
+      <c r="X57" s="71"/>
+      <c r="Y57" s="71"/>
+      <c r="Z57" s="55" t="s">
         <v>381</v>
       </c>
-      <c r="AA57" s="84" t="s">
+      <c r="AA57" s="55" t="s">
         <v>381</v>
       </c>
-      <c r="AB57" s="84" t="s">
+      <c r="AB57" s="55" t="s">
         <v>381</v>
       </c>
-      <c r="AC57" s="84" t="s">
+      <c r="AC57" s="55" t="s">
         <v>379</v>
       </c>
-      <c r="AD57" s="84" t="s">
+      <c r="AD57" s="55" t="s">
         <v>379</v>
       </c>
-      <c r="AE57" s="84" t="s">
+      <c r="AE57" s="55" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="58" spans="21:31" ht="64" customHeight="1">
-      <c r="U58" s="82" t="s">
+      <c r="U58" s="71" t="s">
         <v>432</v>
       </c>
-      <c r="V58" s="82"/>
-      <c r="W58" s="82" t="s">
+      <c r="V58" s="71"/>
+      <c r="W58" s="71" t="s">
         <v>428</v>
       </c>
-      <c r="X58" s="82"/>
-      <c r="Y58" s="82"/>
-      <c r="Z58" s="85" t="s">
+      <c r="X58" s="71"/>
+      <c r="Y58" s="71"/>
+      <c r="Z58" s="56" t="s">
         <v>429</v>
       </c>
-      <c r="AA58" s="85" t="s">
+      <c r="AA58" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="AB58" s="85" t="s">
+      <c r="AB58" s="56" t="s">
         <v>431</v>
       </c>
-      <c r="AC58" s="85" t="s">
+      <c r="AC58" s="56" t="s">
         <v>429</v>
       </c>
-      <c r="AD58" s="85" t="s">
+      <c r="AD58" s="56" t="s">
         <v>430</v>
       </c>
-      <c r="AE58" s="85" t="s">
+      <c r="AE58" s="56" t="s">
         <v>431</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="U58:V58"/>
-    <mergeCell ref="W58:Y58"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="W55:Y55"/>
-    <mergeCell ref="U56:V56"/>
-    <mergeCell ref="W56:Y56"/>
-    <mergeCell ref="U57:V57"/>
-    <mergeCell ref="W57:Y57"/>
-    <mergeCell ref="U52:V52"/>
-    <mergeCell ref="W52:Y52"/>
-    <mergeCell ref="U53:V53"/>
-    <mergeCell ref="W53:Y53"/>
-    <mergeCell ref="U54:V54"/>
-    <mergeCell ref="W54:Y54"/>
-    <mergeCell ref="W48:Y48"/>
-    <mergeCell ref="U49:V49"/>
-    <mergeCell ref="W49:Y49"/>
-    <mergeCell ref="U50:V50"/>
-    <mergeCell ref="W50:Y50"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B24"/>
     <mergeCell ref="U51:V51"/>
     <mergeCell ref="W51:Y51"/>
     <mergeCell ref="N6:N8"/>
@@ -9537,29 +9539,25 @@
     <mergeCell ref="O6:O8"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="U48:V48"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="W48:Y48"/>
+    <mergeCell ref="U49:V49"/>
+    <mergeCell ref="W49:Y49"/>
+    <mergeCell ref="U50:V50"/>
+    <mergeCell ref="W50:Y50"/>
+    <mergeCell ref="U52:V52"/>
+    <mergeCell ref="W52:Y52"/>
+    <mergeCell ref="U53:V53"/>
+    <mergeCell ref="W53:Y53"/>
+    <mergeCell ref="U54:V54"/>
+    <mergeCell ref="W54:Y54"/>
+    <mergeCell ref="U58:V58"/>
+    <mergeCell ref="W58:Y58"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="W55:Y55"/>
+    <mergeCell ref="U56:V56"/>
+    <mergeCell ref="W56:Y56"/>
+    <mergeCell ref="U57:V57"/>
+    <mergeCell ref="W57:Y57"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>